<commit_message>
Handle case when total booking is zero #CRMS-2536
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/partner_penalty_discount.xlsx
+++ b/application/controllers/excel-templates/partner_penalty_discount.xlsx
@@ -43,7 +43,7 @@
     <t>Achieved %</t>
   </si>
   <si>
-    <t>Bookings Failed</t>
+    <t>Bookings Failed %</t>
   </si>
   <si>
     <t>Penalty Amount</t>
@@ -200,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -215,6 +215,9 @@
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -501,10 +504,10 @@
       <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="K2" s="3" t="s">
@@ -519,103 +522,103 @@
       <c r="N2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="13"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="14"/>
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="15" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>